<commit_message>
Begin adding testing scripts and sample software
</commit_message>
<xml_diff>
--- a/hardware/ZRADmini/ZRADminiBOM.xlsx
+++ b/hardware/ZRADmini/ZRADminiBOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eric\Documents\GitHub\ZRAD\hardware\ZRADmini\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CDE31CC-4D9A-4A8C-98CA-2045E2497CC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D75F2B-46A2-4BC5-83BB-201890EF66FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25950" yWindow="750" windowWidth="25950" windowHeight="14730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="236">
   <si>
     <t>Item #</t>
   </si>
@@ -515,9 +515,6 @@
     <t>SPST-NO switch</t>
   </si>
   <si>
-    <t>SW1</t>
-  </si>
-  <si>
     <t>CKN10502TR-ND</t>
   </si>
   <si>
@@ -584,18 +581,6 @@
     <t>JCG402LR-2</t>
   </si>
   <si>
-    <t>MISC</t>
-  </si>
-  <si>
-    <t>Cost</t>
-  </si>
-  <si>
-    <t>Item</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>Low cost recommended antenna - there are several more expensive ones</t>
   </si>
   <si>
@@ -629,9 +614,6 @@
     <t>There are individual tabs for each optional build of ZRAD.</t>
   </si>
   <si>
-    <t>The FULLBOM tab has every possible component included. The other tabs then select only the parts needed for that option.</t>
-  </si>
-  <si>
     <t>Typically do a Save-As of the desired tab as VALUES ONLY either as an .XLSX or .CSV file.</t>
   </si>
   <si>
@@ -650,9 +632,6 @@
     <t>The Test Jig BOM is for the Test Jig which has not been designed yet…</t>
   </si>
   <si>
-    <t>Cost Analysis pie chart:</t>
-  </si>
-  <si>
     <t>Optional</t>
   </si>
   <si>
@@ -701,9 +680,6 @@
     <t>C3</t>
   </si>
   <si>
-    <t>PCB antenna</t>
-  </si>
-  <si>
     <t>SMA Antenna</t>
   </si>
   <si>
@@ -828,6 +804,15 @@
   </si>
   <si>
     <t>Added the RF antenna Tuning components C3, C4, C7</t>
+  </si>
+  <si>
+    <t>SW2</t>
+  </si>
+  <si>
+    <t>Color coded the PCB antenna choices and corrected the LEARN switch from SW1 to SW2</t>
+  </si>
+  <si>
+    <t>The ZRADMiniBOM tab has every possible component included. The other tabs then select only the parts needed for that option.</t>
   </si>
 </sst>
 </file>
@@ -930,12 +915,30 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="14">
@@ -1127,7 +1130,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1190,6 +1193,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -1207,1089 +1222,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.18317054469314931"/>
-          <c:y val="0.16315377534848599"/>
-          <c:w val="0.69358400424666022"/>
-          <c:h val="0.70446752790838318"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:pieChart>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>ZRADminiBOM!$S$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Cost</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-37C4-420C-95B8-F6CB3D3E515D}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000003-37C4-420C-95B8-F6CB3D3E515D}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000005-37C4-420C-95B8-F6CB3D3E515D}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000007-37C4-420C-95B8-F6CB3D3E515D}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000009-37C4-420C-95B8-F6CB3D3E515D}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000B-37C4-420C-95B8-F6CB3D3E515D}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="6"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000D-8C32-493B-A408-99D3E741FCE5}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="7"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="8"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="9"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="10"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="11"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="1"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="1"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="1"/>
-            <c:leaderLines>
-              <c:spPr>
-                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="35000"/>
-                      <a:lumOff val="65000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:round/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:leaderLines>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>ZRADminiBOM!$R$6:$R$17</c:f>
-              <c:strCache>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>Z-Wave MCU/Radio</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>USB2.0 UART</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Antenna</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Bare PCB</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>SMA Verticle</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>SMA Verticle</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>MISC</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>ZRADminiBOM!$S$6:$S$17</c:f>
-              <c:numCache>
-                <c:formatCode>"$"#,##0.00</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>4.8499999999999996</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.34</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4.3548999999999989</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-B7CA-4CA6-B883-B6FA7044AF28}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
-        </c:dLbls>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="25400">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>204786</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCC10EF3-925A-24BB-02D0-A043D5C4F2DA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2555,10 +1487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2568,45 +1500,45 @@
   <sheetData>
     <row r="1" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>174</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="J5" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -2627,7 +1559,7 @@
         <v>45406</v>
       </c>
       <c r="B14" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -2635,7 +1567,7 @@
         <v>45455</v>
       </c>
       <c r="B15" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -2643,7 +1575,7 @@
         <v>45610</v>
       </c>
       <c r="B16" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2651,7 +1583,15 @@
         <v>45644</v>
       </c>
       <c r="B17" t="s">
-        <v>240</v>
+        <v>232</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>45657</v>
+      </c>
+      <c r="B18" t="s">
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -2667,8 +1607,8 @@
   <dimension ref="A1:S49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2730,7 +1670,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>9</v>
@@ -2774,7 +1714,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>9</v>
@@ -2786,7 +1726,7 @@
         <v>34</v>
       </c>
       <c r="F3" s="32" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G3" s="11">
         <v>1</v>
@@ -2804,9 +1744,6 @@
       <c r="K3" s="13">
         <f t="shared" ref="K3:K41" si="1">MAX($M$2*G3-J3,0)</f>
         <v>5</v>
-      </c>
-      <c r="R3" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -2815,19 +1752,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>34</v>
       </c>
       <c r="F4" s="32" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="G4" s="11">
         <v>0</v>
@@ -2847,7 +1784,7 @@
         <v>0</v>
       </c>
       <c r="M4" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -2887,12 +1824,6 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="R5" t="s">
-        <v>161</v>
-      </c>
-      <c r="S5" t="s">
-        <v>160</v>
-      </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="22">
@@ -2932,16 +1863,9 @@
         <v>4</v>
       </c>
       <c r="M6" t="s">
-        <v>164</v>
-      </c>
-      <c r="R6" t="str">
-        <f>$D$2</f>
-        <v>Z-Wave MCU/Radio</v>
-      </c>
-      <c r="S6" s="2">
-        <f>I2</f>
-        <v>4.8499999999999996</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="S6" s="2"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="22">
@@ -2958,7 +1882,7 @@
         <v>41</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="F7" s="29" t="s">
         <v>44</v>
@@ -2980,14 +1904,7 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="R7" t="str">
-        <f>$D$3</f>
-        <v>USB2.0 UART</v>
-      </c>
-      <c r="S7" s="2">
-        <f>I3</f>
-        <v>2.34</v>
-      </c>
+      <c r="S7" s="2"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="22">
@@ -3004,7 +1921,7 @@
         <v>47</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="F8" s="29" t="s">
         <v>46</v>
@@ -3026,14 +1943,7 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="R8" t="str">
-        <f>$D$43</f>
-        <v>Antenna</v>
-      </c>
-      <c r="S8" s="2">
-        <f>I43</f>
-        <v>0</v>
-      </c>
+      <c r="S8" s="2"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="22">
@@ -3050,7 +1960,7 @@
         <v>49</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="F9" s="29" t="s">
         <v>50</v>
@@ -3072,14 +1982,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R9" t="str">
-        <f>$D$42</f>
-        <v>Bare PCB</v>
-      </c>
-      <c r="S9" s="2">
-        <f>I42</f>
-        <v>1</v>
-      </c>
+      <c r="S9" s="2"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="22">
@@ -3096,12 +1999,12 @@
         <v>52</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="F10" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="42">
         <v>0</v>
       </c>
       <c r="H10" s="12">
@@ -3118,17 +2021,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M10" t="s">
-        <v>199</v>
-      </c>
-      <c r="R10" t="str">
-        <f>$D$24</f>
-        <v>SMA Verticle</v>
-      </c>
-      <c r="S10" s="2">
-        <f>I24</f>
-        <v>0</v>
-      </c>
+      <c r="M10" s="43" t="s">
+        <v>191</v>
+      </c>
+      <c r="S10" s="2"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="22">
@@ -3136,21 +2032,21 @@
         <v>10</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>239</v>
-      </c>
-      <c r="G11" s="11">
+        <v>231</v>
+      </c>
+      <c r="G11" s="40">
         <v>1</v>
       </c>
       <c r="H11" s="12">
@@ -3162,11 +2058,11 @@
       </c>
       <c r="J11" s="10"/>
       <c r="K11" s="13"/>
-      <c r="M11" t="s">
-        <v>219</v>
+      <c r="M11" s="44" t="s">
+        <v>211</v>
       </c>
       <c r="O11" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="S11" s="2"/>
     </row>
@@ -3176,21 +2072,21 @@
         <v>11</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="F12" s="29" t="s">
-        <v>226</v>
-      </c>
-      <c r="G12" s="11">
+        <v>218</v>
+      </c>
+      <c r="G12" s="40">
         <v>1</v>
       </c>
       <c r="H12" s="12">
@@ -3199,7 +2095,7 @@
       <c r="I12" s="12"/>
       <c r="J12" s="10"/>
       <c r="K12" s="13"/>
-      <c r="M12" t="str">
+      <c r="M12" s="44" t="str">
         <f>M11</f>
         <v>US PCB antenna</v>
       </c>
@@ -3211,21 +2107,21 @@
         <v>12</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>229</v>
-      </c>
-      <c r="G13" s="11">
+        <v>221</v>
+      </c>
+      <c r="G13" s="40">
         <v>1</v>
       </c>
       <c r="H13" s="12">
@@ -3234,7 +2130,7 @@
       <c r="I13" s="12"/>
       <c r="J13" s="10"/>
       <c r="K13" s="13"/>
-      <c r="M13" t="str">
+      <c r="M13" s="44" t="str">
         <f>M12</f>
         <v>US PCB antenna</v>
       </c>
@@ -3246,21 +2142,21 @@
         <v>13</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>237</v>
-      </c>
-      <c r="G14" s="11">
+        <v>229</v>
+      </c>
+      <c r="G14" s="41">
         <v>1</v>
       </c>
       <c r="H14" s="12">
@@ -3269,8 +2165,8 @@
       <c r="I14" s="12"/>
       <c r="J14" s="10"/>
       <c r="K14" s="13"/>
-      <c r="M14" t="s">
-        <v>220</v>
+      <c r="M14" s="45" t="s">
+        <v>212</v>
       </c>
       <c r="S14" s="2"/>
     </row>
@@ -3280,21 +2176,21 @@
         <v>14</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="G15" s="11">
+        <v>223</v>
+      </c>
+      <c r="G15" s="41">
         <v>2</v>
       </c>
       <c r="H15" s="12">
@@ -3303,7 +2199,7 @@
       <c r="I15" s="12"/>
       <c r="J15" s="10"/>
       <c r="K15" s="13"/>
-      <c r="M15" t="str">
+      <c r="M15" s="45" t="str">
         <f>M14</f>
         <v>EU PCB Antenna</v>
       </c>
@@ -3314,49 +2210,23 @@
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="B16" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="G16" s="11">
-        <v>1</v>
-      </c>
-      <c r="H16" s="12">
-        <v>0.03</v>
-      </c>
+      <c r="B16" s="26"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="12"/>
       <c r="I16" s="12">
         <f t="shared" ref="I16" si="4">H16*G16</f>
-        <v>0.03</v>
-      </c>
-      <c r="J16" s="10">
-        <v>40</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J16" s="10"/>
       <c r="K16" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M16" t="s">
-        <v>198</v>
-      </c>
-      <c r="R16" t="str">
-        <f>$D$24</f>
-        <v>SMA Verticle</v>
-      </c>
-      <c r="S16" s="2">
-        <f>I25</f>
-        <v>0</v>
-      </c>
+      <c r="S16" s="2"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="22">
@@ -3395,13 +2265,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="R17" t="s">
-        <v>159</v>
-      </c>
-      <c r="S17" s="2">
-        <f>I47-SUM(S6:S10)</f>
-        <v>4.3548999999999989</v>
-      </c>
+      <c r="S17" s="2"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="22">
@@ -3418,7 +2282,7 @@
         <v>58</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F18" s="10" t="s">
         <v>60</v>
@@ -3440,13 +2304,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R18" t="s">
-        <v>162</v>
-      </c>
-      <c r="S18" s="2">
-        <f>SUM(S6:S17)</f>
-        <v>12.544899999999998</v>
-      </c>
+      <c r="S18" s="2"/>
     </row>
     <row r="19" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="22">
@@ -3463,7 +2321,7 @@
         <v>62</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="F19" s="10" t="s">
         <v>63</v>
@@ -3501,7 +2359,7 @@
         <v>65</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="F20" s="14" t="s">
         <v>66</v>
@@ -3618,7 +2476,7 @@
         <v>79</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F23" s="10" t="s">
         <v>77</v>
@@ -3694,7 +2552,7 @@
         <v>88</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F25" s="10" t="s">
         <v>89</v>
@@ -3735,7 +2593,7 @@
         <v>93</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="F26" s="10" t="s">
         <v>94</v>
@@ -3773,7 +2631,7 @@
         <v>96</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F27" s="10" t="s">
         <v>98</v>
@@ -3811,7 +2669,7 @@
         <v>102</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="F28" s="10" t="s">
         <v>100</v>
@@ -3887,7 +2745,7 @@
         <v>106</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F30" s="10" t="s">
         <v>107</v>
@@ -3925,7 +2783,7 @@
         <v>109</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="F31" s="10" t="s">
         <v>110</v>
@@ -3963,7 +2821,7 @@
         <v>113</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="F32" s="10" t="s">
         <v>114</v>
@@ -4001,7 +2859,7 @@
         <v>116</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="F33" s="10" t="s">
         <v>117</v>
@@ -4039,7 +2897,7 @@
         <v>119</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="F34" s="10" t="s">
         <v>120</v>
@@ -4077,7 +2935,7 @@
         <v>122</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="F35" s="10" t="s">
         <v>123</v>
@@ -4115,7 +2973,7 @@
         <v>125</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="F36" s="10" t="s">
         <v>126</v>
@@ -4153,7 +3011,7 @@
         <v>128</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="F37" s="10" t="s">
         <v>129</v>
@@ -4191,7 +3049,7 @@
         <v>131</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="F38" s="10" t="s">
         <v>132</v>
@@ -4229,10 +3087,10 @@
         <v>135</v>
       </c>
       <c r="E39" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="F39" s="10" t="s">
         <v>136</v>
-      </c>
-      <c r="F39" s="10" t="s">
-        <v>137</v>
       </c>
       <c r="G39" s="11">
         <v>0</v>
@@ -4252,7 +3110,7 @@
         <v>0</v>
       </c>
       <c r="M39" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -4261,19 +3119,19 @@
         <v>39</v>
       </c>
       <c r="B40" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="C40" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="C40" s="10" t="s">
+      <c r="D40" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="D40" s="10" t="s">
+      <c r="E40" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="E40" s="10" t="s">
+      <c r="F40" s="10" t="s">
         <v>142</v>
-      </c>
-      <c r="F40" s="10" t="s">
-        <v>143</v>
       </c>
       <c r="G40" s="11">
         <v>0</v>
@@ -4293,7 +3151,7 @@
         <v>0</v>
       </c>
       <c r="M40" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
@@ -4302,17 +3160,17 @@
         <v>40</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E41" s="10"/>
       <c r="F41" s="10" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="G41" s="11">
         <v>1</v>
@@ -4333,11 +3191,11 @@
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="22"/>
       <c r="B42" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C42" s="10"/>
       <c r="D42" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E42" s="15"/>
       <c r="F42" s="10"/>
@@ -4354,21 +3212,21 @@
       <c r="J42" s="10"/>
       <c r="K42" s="13"/>
       <c r="M42" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C43" s="10"/>
       <c r="D43" s="10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E43" s="10"/>
       <c r="F43" s="26" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G43" s="11">
         <v>0</v>
@@ -4383,7 +3241,7 @@
       <c r="J43" s="10"/>
       <c r="K43" s="13"/>
       <c r="M43" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
@@ -4391,7 +3249,7 @@
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
       <c r="D44" s="10" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="E44" s="10"/>
       <c r="F44" s="10"/>
@@ -4406,7 +3264,7 @@
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
       <c r="D45" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E45" s="10"/>
       <c r="F45" s="10"/>
@@ -4421,7 +3279,7 @@
       <c r="B46" s="10"/>
       <c r="C46" s="10"/>
       <c r="D46" s="10" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E46" s="10"/>
       <c r="F46" s="35"/>
@@ -4438,18 +3296,18 @@
       <c r="D47" s="10"/>
       <c r="E47" s="10"/>
       <c r="F47" s="37" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="G47" s="38"/>
       <c r="H47" s="39"/>
       <c r="I47" s="34">
         <f>SUM(I2:I46)</f>
-        <v>12.544899999999998</v>
+        <v>12.514899999999997</v>
       </c>
       <c r="J47" s="10"/>
       <c r="K47" s="13"/>
       <c r="M47" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
@@ -4465,7 +3323,7 @@
       <c r="J48" s="10"/>
       <c r="K48" s="13"/>
       <c r="M48" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
@@ -4481,7 +3339,7 @@
       <c r="J49" s="17"/>
       <c r="K49" s="20"/>
       <c r="M49" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -4498,17 +3356,15 @@
     <hyperlink ref="B19" r:id="rId10" display="https://www.digikey.com/en/products/detail/murata-electronics/GRM21BR71C475KE51L/6606095" xr:uid="{D1C9B504-EA11-47B0-A380-66685325C2A3}"/>
     <hyperlink ref="B20" r:id="rId11" display="https://www.digikey.com/en/products/detail/murata-electronics/GCM188L81H104KA57D/2591908" xr:uid="{CF280619-1A25-4425-9524-CC71C1A3F4D8}"/>
     <hyperlink ref="F43" r:id="rId12" display="https://www.digikey.com/en/products/detail/jc-antenna/JCG402LR-2/15814458" xr:uid="{C038367E-887A-4E6B-BA17-618664AFA725}"/>
-    <hyperlink ref="B16" r:id="rId13" display="https://www.digikey.com/en/products/detail/murata-electronics/GJM1555C1H470FB01D/7363120" xr:uid="{C18DB824-9FFB-4EE0-9100-4F6C84ED2198}"/>
-    <hyperlink ref="B12" r:id="rId14" display="https://www.digikey.com/en/products/detail/murata-electronics/GCM1555C1H3R0BA16D/6606050" xr:uid="{E2209988-C899-40B5-982D-796A10170EA8}"/>
-    <hyperlink ref="B13" r:id="rId15" display="https://www.digikey.com/en/products/detail/murata-electronics/GRM1555C1H3R3CA01D/3693848" xr:uid="{6383CF9A-11AE-4831-BF0D-E760188EFB66}"/>
-    <hyperlink ref="B15" r:id="rId16" display="https://www.digikey.com/en/products/detail/murata-electronics/GRM1555C1H4R7CA01D/3175193" xr:uid="{3A64D669-6C78-4F75-BF0C-BD9A52BAB7AC}"/>
-    <hyperlink ref="B14" r:id="rId17" display="https://www.digikey.com/en/products/detail/murata-electronics/LQW18AN27NG00D/2594997" xr:uid="{E00C8425-EA9F-44C7-AF05-17F3B46B1A78}"/>
-    <hyperlink ref="B11" r:id="rId18" display="https://www.digikey.com/en/products/detail/murata-electronics/LQW15AN22NG00D/2594872" xr:uid="{3A8EED4D-FAE0-4D34-A6A5-4D3623F9D598}"/>
+    <hyperlink ref="B12" r:id="rId13" display="https://www.digikey.com/en/products/detail/murata-electronics/GCM1555C1H3R0BA16D/6606050" xr:uid="{E2209988-C899-40B5-982D-796A10170EA8}"/>
+    <hyperlink ref="B13" r:id="rId14" display="https://www.digikey.com/en/products/detail/murata-electronics/GRM1555C1H3R3CA01D/3693848" xr:uid="{6383CF9A-11AE-4831-BF0D-E760188EFB66}"/>
+    <hyperlink ref="B15" r:id="rId15" display="https://www.digikey.com/en/products/detail/murata-electronics/GRM1555C1H4R7CA01D/3175193" xr:uid="{3A64D669-6C78-4F75-BF0C-BD9A52BAB7AC}"/>
+    <hyperlink ref="B14" r:id="rId16" display="https://www.digikey.com/en/products/detail/murata-electronics/LQW18AN27NG00D/2594997" xr:uid="{E00C8425-EA9F-44C7-AF05-17F3B46B1A78}"/>
+    <hyperlink ref="B11" r:id="rId17" display="https://www.digikey.com/en/products/detail/murata-electronics/LQW15AN22NG00D/2594872" xr:uid="{3A8EED4D-FAE0-4D34-A6A5-4D3623F9D598}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="92" orientation="portrait" r:id="rId19"/>
-  <drawing r:id="rId20"/>
-  <legacyDrawing r:id="rId21"/>
+  <pageSetup scale="92" orientation="portrait" r:id="rId18"/>
+  <legacyDrawing r:id="rId19"/>
 </worksheet>
 </file>
 
@@ -4621,7 +3477,7 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -4654,7 +3510,7 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -5515,7 +4371,7 @@
       </c>
       <c r="E33" t="str">
         <f>ZRADminiBOM!E39</f>
-        <v>SW1</v>
+        <v>SW2</v>
       </c>
       <c r="F33" t="str">
         <f>ZRADminiBOM!F39</f>
@@ -5716,7 +4572,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A36" sqref="A36:XFD38"/>
     </sheetView>
   </sheetViews>
@@ -5820,7 +4676,7 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -6680,7 +5536,7 @@
       </c>
       <c r="E32" t="str">
         <f>ZRADminiBOM!E39</f>
-        <v>SW1</v>
+        <v>SW2</v>
       </c>
       <c r="F32" t="str">
         <f>ZRADminiBOM!F39</f>
@@ -6719,7 +5575,7 @@
         <v>1</v>
       </c>
       <c r="I33" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -6930,7 +5786,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -6940,7 +5796,7 @@
       </c>
       <c r="B7" s="26"/>
       <c r="D7" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -6950,7 +5806,7 @@
       </c>
       <c r="B8" s="26"/>
       <c r="D8" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -6998,12 +5854,12 @@
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>